<commit_message>
C# Studing material updated
</commit_message>
<xml_diff>
--- a/C#.xlsx
+++ b/C#.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="371">
   <si>
     <t>Expalnation</t>
     <phoneticPr fontId="1"/>
@@ -2264,13 +2264,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Classes and Objects</t>
-  </si>
-  <si>
-    <t>Classes and Objects</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Everything in C# is associated with classes and objects, along with its attributes and methods.</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -2349,10 +2342,1146 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
+    <t>Class Members</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Fields(Attributes) and methods inside classes are often referred to as "Class Members"</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>// The class
+class MyClass
+{
+  // Class members
+  string color = "red";        // field
+  int maxSpeed = 200;          // field
+  public void fullThrottle()   // method
+  {
+    Console.WriteLine("The car is going as fast as it can!");
+  }
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Fields</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> variables inside a class are called fields, and that you can access them by creating an object of the class, and by using the dot syntax (.).</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>class Car 
+{
+  string color = "red";
+  int maxSpeed = 200;
+  static void Main(string[] args)
+  {
+    Car myObj = new Car();
+    Console.WriteLine(myObj.color);
+    Console.WriteLine(myObj.maxSpeed);
+  }
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>You can also leave the fields blank, and modify them when creating the object</t>
+  </si>
+  <si>
+    <t>class Car 
+{
+  string color;
+  int maxSpeed;
+  static void Main(string[] args)
+  {
+    Car myObj = new Car();
+    myObj.color = "red";
+    myObj.maxSpeed = 200;
+    Console.WriteLine(myObj.color);
+    Console.WriteLine(myObj.maxSpeed);
+  }
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>This is especially useful when creating multiple objects of one class</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>class Car 
+{
+  string model;
+  string color;
+  int year;
+  static void Main(string[] args)
+  {
+    Car Ford = new Car();
+    Ford.model = "Mustang";
+    Ford.color = "red";
+    Ford.year = 1969;
+    Car Opel = new Car();
+    Opel.model = "Astra";
+    Opel.color = "white";
+    Opel.year = 2005;
+    Console.WriteLine(Ford.model);
+    Console.WriteLine(Opel.model);
+  }
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Object Methods</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>methods are used to perform certain actions.
+Methods normally belongs to a class, and they define how an object of a class behaves.
+Just like with fields, you can access methods with the dot syntax. However, note that the method must be public. And remember that we use the name of the method followed by two parantheses () and a semicolon ; to call (execute) the method</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>class Car 
+{
+  string color;                 // field
+  int maxSpeed;                 // field
+  public void fullThrottle()    // method
+  {
+    Console.WriteLine("The car is going as fast as it can!"); 
+  }
+  static void Main(string[] args)
+  {
+    Car myObj = new Car();
+    myObj.fullThrottle();  // Call the method
+  }
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Use Multiple Classes</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>we can use multiple classes for better organization (one for fields and methods, and another one for execution). This is recommended</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Constructors</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>// Create a Car class
+class Car
+{
+  public string model;  // Create a field
+  // Create a class constructor for the Car class
+  public Car()
+  {
+    model = "Mustang"; // Set the initial value for model
+  }
+  static void Main(string[] args)
+  {
+    Car Ford = new Car();  // Create an object of the Car Class (this will call the constructor)
+    Console.WriteLine(Ford.model);  // Print the value of model
+  }
+}
+// Outputs "Mustang"</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A constructor is a special method that is used to initialize objects. The advantage of a constructor, is that it is called when an object of a class is created. It can be used to set initial values for fields
+the constructor name </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>must match the class name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, and it cannot have a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>return type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (like void or int).
+ the constructor is called when the object is created.
+All classes have constructors by default: if you do not create a class constructor yourself, C# creates one for you. However, then you are not able to set initial values for fields.
+Constructors save time! Take a look at the last example on this page to really understand why.</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Constructor Parameters</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Constructors can also take parameters, which is used to initialize fields.
+The following example adds a string modelName parameter to the constructor. Inside the constructor we set model to modelName (model=modelName). When we call the constructor, we pass a parameter to the constructor ("Mustang"), which will set the value of model to "Mustang"</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>class Car
+{
+  public string model;
+  // Create a class constructor with a parameter
+  public Car(string modelName)
+  {
+    model = modelName;
+  }
+  static void Main(string[] args)
+  {
+    Car Ford = new Car("Mustang");
+    Console.WriteLine(Ford.model);
+  }
+}
+// Outputs "Mustang"</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>class Car
+{
+  public string model;
+  public string color;
+  public int year;
+  // Create a class constructor with multiple parameters
+  public Car(string modelName, string modelColor, int modelYear)
+  {
+    model = modelName;
+    color = modelColor;
+    year = modelYear;
+  }
+  static void Main(string[] args)
+  {
+    Car Ford = new Car("Mustang", "Red", 1969);
+    Console.WriteLine(Ford.color + " " + Ford.year + " " + Ford.model);
+  }
+}
+// Outputs Red 1969 Mustang</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>can have as many parameters as you want
+Tip: Just like other methods, constructors can be overloaded by using different numbers of parameters.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Constructors Save Time</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Without constructor:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+class Program
+{
+  static void Main(string[] args)
+  {
+    Car Ford = new Car();
+    Ford.model = "Mustang";
+    Ford.color = "red";
+    Ford.year = 1969;
+    Car Opel = new Car();
+    Opel.model = "Astra";
+    Opel.color = "white";
+    Opel.year = 2005;
+    Console.WriteLine(Ford.model);
+    Console.WriteLine(Opel.model);
+  }
+}</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Classes and Objects</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Access Modifiers</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>The public keyword is an access modifier, which is used to set the access level/visibility for classes, fields, methods and properties.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Private Modifier</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>class Car
+ {
+  private string model = "Mustang";
+  static void Main(string[] args)
+  {
+    Car myObj = new Car();
+    Console.WriteLine(myObj.model);
+  }
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>If you declare a field with a private access modifier, it can only be accessed within the same class
+If you try to access it outside the class, an error will occur</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Public Modifier</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>If you declare a field with a public access modifier, it is accessible for all classes</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>class Car
+{
+  public string model = "Mustang";
+}
+class Program
+{
+  static void Main(string[] args)
+  {
+    Car myObj = new Car();
+    Console.WriteLine(myObj.model);
+  }
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Why Access Modifiers?</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>To control the visibility of class members (the security level of each individual class and class member).
+To achieve "Encapsulation" - which is the process of making sure that "sensitive" data is hidden from users. This is done by declaring fields as private</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Properties (Get and Set)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Properties and Encapsulation</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Properties</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>You learned from the previous chapter that private variables can only be accessed within the same class (an outside class has no access to it). However, sometimes we need to access them - and it can be done with properties.
+A property is like a combination of a variable and a method, and it has two methods: a get and a set method</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>we can use the Name property to access and update the private field of the Person class</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>class Person
+{
+  private string name; // field
+  public string Name   // property
+  {
+    get { return name; }
+    set { name = value; }
+  }
+}
+class Program
+{
+  static void Main(string[] args)
+  {
+    Person myObj = new Person();
+    myObj.Name = "Liam";
+    Console.WriteLine(myObj.Name);
+  }
+}
+// Outputs Liam</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Automatic Properties (Short Hand)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>C# also provides a way to use short-hand / automatic properties, where you do not have to define the field for the property, and you only have to write get; and set; inside the property.
+The following example will produce the same result as the example above. The only difference is that there is less code</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>class Person
+{
+  public string Name  // property
+  { get; set; }
+}
+class Program
+{
+  static void Main(string[] args)
+  {
+    Person myObj = new Person();
+    myObj.Name = "Liam";
+    Console.WriteLine(myObj.Name);
+  }
+}
+// Outputs Liam</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Inheritance</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Inheritance (Derived and Base Class)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>In C#, it is possible to inherit fields and methods from one class to another. We group the "inheritance concept" into two categories:
+Derived Class (child) - the class that inherits from another class
+Base Class (parent) - the class being inherited from
+To inherit from a class, use the</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> :</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> symbol.
+In the example below, the Car class (child) inherits the fields and methods from the Vehicle class (parent)</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>class Vehicle  // base class (parent) 
+{
+  public string brand = "Ford";  // Vehicle field
+  public void honk()             // Vehicle method 
+  {                    
+    Console.WriteLine("Tuut, tuut!");
+  }
+}
+class Car : Vehicle  // derived class (child)
+{
+  public string modelName = "Mustang";  // Car field
+}
+class Program
+{
+  static void Main(string[] args)
+  {
+    // Create a myCar object
+    Car myCar = new Car();
+    // Call the honk() method (From the Vehicle class) on the myCar object
+    myCar.honk();
+    // Display the value of the brand field (from the Vehicle class) and the value of the modelName from the Car class
+    Console.WriteLine(myCar.brand + " " + myCar.modelName);
+  }
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Why And When To Use "Inheritance"?</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>It is useful for code reusability: reuse fields and methods of an existing class when you create a new class.
+Polymorphism, which uses inherited methods to perform different tasks.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>The sealed Keyword</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>If you don't want other classes to inherit from a class, use the sealed keyword</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Polymorphism</t>
+  </si>
+  <si>
+    <t>Polymorphism and Overriding Methods</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Polymorphism means "many forms", and it occurs when we have many classes that are related to each other by inheritance.
+Like we specified in the previous chapter; Inheritance lets us inherit fields and methods from another class. Polymorphism uses those methods to perform different tasks. This allows us to perform a single action in different ways.
+For example, think of a base class called Animal that has a method called animalSound(). Derived classes of Animals could be Pigs, Cats, Dogs, Birds - And they also have their own implementation of an animal sound (the pig oinks, and the cat meows, etc.):</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>class Animal  // Base class (parent) 
+{
+  public void animalSound() 
+  {
+    Console.WriteLine("The animal makes a sound");
+  }
+}
+class Pig : Animal  // Derived class (child) 
+{
+  public void animalSound() 
+  {
+    Console.WriteLine("The pig says: wee wee");
+  }
+}
+class Dog : Animal  // Derived class (child) 
+{
+  public void animalSound() 
+  {
+    Console.WriteLine("The dog says: bow wow");
+  }
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Now we can create Pig and Dog objects and call the animalSound() method on both of them</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>class Animal  // Base class (parent) 
+{
+  public void animalSound() 
+  {Console.WriteLine("The animal makes a sound");}
+}
+class Pig : Animal  // Derived class (child) 
+{
+  public void animalSound() 
+  {Console.WriteLine("The pig says: wee wee"); }
+}
+class Dog : Animal  // Derived class (child) 
+{
+  public void animalSound() 
+  {Console.WriteLine("The dog says: bow wow"); }
+}
+class Program 
+{
+  static void Main(string[] args) 
+  {
+    Animal myAnimal = new Animal();  // Create a Animal object
+    Animal myPig = new Pig();  // Create a Pig object
+    Animal myDog = new Dog();  // Create a Dog object
+    myAnimal.animalSound();
+    myPig.animalSound();
+    myDog.animalSound();
+  }
+}
+//outputs
+The animal makes a sound
+The animal makes a sound
+The animal makes a sound</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>class Animal  // Base class (parent) 
+{
+  public virtual void animalSound() 
+  {
+    Console.WriteLine("The animal makes a sound");
+  }
+}
+class Pig : Animal  // Derived class (child) 
+{
+  public override void animalSound() 
+  {
+    Console.WriteLine("The pig says: wee wee");
+  }
+}
+class Dog : Animal  // Derived class (child) 
+{
+  public override void animalSound() 
+  {
+    Console.WriteLine("The dog says: bow wow");
+  }
+}
+class Program 
+{
+  static void Main(string[] args) 
+  {
+    Animal myAnimal = new Animal();  // Create a Animal object
+    Animal myPig = new Pig();  // Create a Pig object
+    Animal myDog = new Dog();  // Create a Dog object
+    myAnimal.animalSound();
+    myPig.animalSound();
+    myDog.animalSound();
+  }
+}
+//Outputs 
+The animal makes a sound
+The pig says: wee wee
+The dog says: bow wow</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The output from the example above was probably not what you expected. That is because the base class method overrides the derived class method, when they share the same name.
+However, C# provides an option to override the base class method, by adding the virtual keyword to the method inside the base class, and by using the override keyword for each derived class methods:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Why And When To Use "Inheritance" and "Polymorphism"?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+It is useful for code reusability: reuse fields and methods of an existing class when you create a new class.</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Abstraction</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Abstract Classes and Methods</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Data abstraction is the process of hiding certain details and showing only essential information to the user.
+Abstraction can be achieved with either abstract classes or interfaces
+The abstract keyword is used for classes and methods:
+Abstract class: is a restricted class that cannot be used to create objects (to access it, it must be inherited from another class).
+Abstract method: can only be used in an abstract class, and it does not have a body. The body is provided by the derived class (inherited from)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>// Abstract class
+abstract class Animal
+{
+  // Abstract method (does not have a body)
+  public abstract void animalSound();
+  // Regular method
+  public void sleep()
+  {
+    Console.WriteLine("Zzz");
+  }
+}
+// Derived class (inherit from Animal)
+class Pig : Animal
+{
+  public override void animalSound()
+  {
+    // The body of animalSound() is provided here
+    Console.WriteLine("The pig says: wee wee");
+  }
+}
+class Program
+{
+  static void Main(string[] args)
+  {
+    Pig myPig = new Pig(); // Create a Pig object
+    myPig.animalSound();  // Call the abstract method
+    myPig.sleep();  // Call the regular method
+  }
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Why And When To Use Abstract Classes and Methods?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>To achieve security - hide certain details and only show the important details of an object.
+Note: Abstraction can also be achieved with Interfaces</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Interface</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Interfaces
+Another way to achieve abstraction in C#, is with interfaces.
+An interface is a completely "abstract class", which can only contain abstract methods and properties (with empty bodies)
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">To access the interface methods, the interface must be "implemented" (kinda like inherited) by another class. To implement an interface, use the : symbol (just like with inheritance). The body of the interface method is provided by the "implement" class. Note that you do not have to use the override keyword when implementing an interface
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Why And When To Use Interfaces?</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+1) To achieve security - hide certain details and only show the important details of an object (interface).
+2) C# does not support "multiple inheritance" (a class can only inherit from one base class). However, it can be achieved with interfaces, because the class can implement multiple interfaces. Note: To implement multiple interfaces, separate them with a comma (see example below).</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>// Interface
+interface IAnimal 
+{
+  void animalSound(); // interface method (does not have a body)
+}
+// Pig "implements" the IAnimal interface
+class Pig : IAnimal 
+{
+  public void animalSound() 
+  {
+    // The body of animalSound() is provided here
+    Console.WriteLine("The pig says: wee wee");
+  }
+}
+class Program 
+{
+  static void Main(string[] args) 
+  {
+    Pig myPig = new Pig();  // Create a Pig object
+    myPig.animalSound();
+  }
+}
+Notes on Interfaces:
+Like abstract classes, interfaces cannot be used to create objects (in the example above, it is not possible to create an "IAnimal" object in the Program class)
+Interface methods do not have a body - the body is provided by the "implement" class
+On implementation of an interface, you must override all of its methods
+Interfaces can contain properties and methods, but not fields/variables
+Interface members are by default abstract and public
+An interface cannot contain a constructor (as it cannot be used to create objects)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Multiple Interfaces</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>To implement multiple interfaces, separate them with a comma</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>interface IFirstInterface 
+{
+  void myMethod(); // interface method
+}
+interface ISecondInterface 
+{
+  void myOtherMethod(); // interface method
+}
+// Implement multiple interfaces
+class DemoClass : IFirstInterface, ISecondInterface 
+{
+  public void myMethod() 
+  {
+    Console.WriteLine("Some text..");
+  }
+  public void myOtherMethod() 
+  {
+    Console.WriteLine("Some other text...");
+  }
+}
+class Program 
+{
+  static void Main(string[] args)
+  {
+    DemoClass myObj = new DemoClass();
+    myObj.myMethod();
+    myObj.myOtherMethod();
+  }
+}</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Enum</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">An enum is a special "class" that represents a group of constants (unchangeable/read-only variables).
+To create an enum, use the enum keyword (instead of class or interface), and separate the enum items with a comma
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Enum is short for "enumerations", which means "specifically listed".</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Enum inside a Class</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>You can also have an enum inside a class</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>class Program
+{
+  enum Level
+  {
+    Low,
+    Medium,
+    High
+  }
+  static void Main(string[] args)
+  {
+    Level myVar = Level.Medium;
+    Console.WriteLine(myVar);
+  }
+}
+//Outputs Medium</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Enum Values</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>By default, the first item of an enum has the value 0. The second has the value 1, and so on.
+To get the integer value from an item, you must explicitly convert the item to an int</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>enum Months
+{
+  January,    // 0
+  February,   // 1
+  March,      // 2
+  April,      // 3
+  May,        // 4
+  June,       // 5
+  July        // 6
+}
+static void Main(string[] args)
+{
+  int myNum = (int) Months.April;
+  Console.WriteLine(myNum);
+}
+//Outputs 3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Enum in a Switch Statement</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>enum Level 
+{
+  Low,
+  Medium,
+  High
+}
+static void Main(string[] args) 
+{
+  Level myVar = Level.Medium;
+  switch(myVar) 
+  {
+    case Level.Low:
+      Console.WriteLine("Low level");
+      break;
+    case Level.Medium:
+       Console.WriteLine("Medium level");
+      break;
+    case Level.High:
+      Console.WriteLine("High level");
+      break;
+  }
+}
+//outputs Medium level</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Enums are often used in switch statements to check for corresponding values
+Why And When To Use Enums?
+Use enums when you have values that you know aren't going to change, like month days, days, colors, deck of cards, etc.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Files</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Working With Files</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>The File class from the System.IO namespace, allows us to work with files
+using System.IO;  // include the System.IO namespace
+File.SomeFileMethod();  // use the file class with methods</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>AppendText() --&gt; Appends text at the end of an existing file
+Copy()             --&gt; Copies a file
+Create()          --&gt; Creates or overwrites a file
+Delete()          --&gt; Deletes a file
+Exists()           --&gt; Tests whether the file exists
+ReadAllText() --&gt; Reads the contents of a file
+Replace()        --&gt; Replaces the contents of a file with the contents of another file
+WriteAllText()  --&gt; Creates a new file and writes the contents to it. If the file already exists, it will be overwritten.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Write To a File and Read It</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>In the following example, we use the WriteAllText() method to create a file named "filename.txt" and write some content to it. Then we use the ReadAllText() method to read the contents of the file:</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>using System.IO;  // include the System.IO namespace
+string writeText = "Hello World!";  // Create a text string
+File.WriteAllText("filename.txt", writeText);  // Create a file and write the content of writeText to it
+string readText = File.ReadAllText("filename.txt");  // Read the contents of the file
+Console.WriteLine(readText);  // Output the content</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Exceptions - Try..Catch</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Exceptions</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>C# try and catch</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>When executing C# code, different errors can occur: coding errors made by the programmer, errors due to wrong input, or other unforeseeable things.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>When an error occurs, C# will normally stop and generate an error message. The technical term for this is: C# will throw an exception (throw an error).</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>The try statement allows you to define a block of code to be tested for errors while it is being executed.
+The catch statement allows you to define a block of code to be executed, if an error occurs in the try block.
+The try and catch keywords come in pairs</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>This will generate an error, because myNumbers[10] does not exist</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.
+int[] myNumbers = {1, 2, 3};
+Console.WriteLine(myNumbers[10]); // error!</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>try
+{
+  int[] myNumbers = {1, 2, 3};
+  Console.WriteLine(myNumbers[10]);
+}
+catch (Exception e)
+{
+  Console.WriteLine(e.Message);
+}
+//outputs Index was outside the bounds of the array.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>You can also output your own error message</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>try
+{
+  int[] myNumbers = {1, 2, 3};
+  Console.WriteLine(myNumbers[10]);
+}
+catch (Exception e)
+{
+  Console.WriteLine("Something went wrong.");
+}
+//Outputs Something went wrong.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Finally</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>The finally statement lets you execute code, after try...catch, regardless of the result</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>try
+{
+  int[] myNumbers = {1, 2, 3};
+  Console.WriteLine(myNumbers[10]);
+}
+catch (Exception e)
+{
+  Console.WriteLine("Something went wrong.");
+}
+finally
+{
+  Console.WriteLine("The 'try catch' is finished.");
+}
+//outputs The 'try catch' is finished.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>The throw keyword</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>The throw statement allows you to create a custom error.
+The throw statement is used together with an exception class. There are many exception classes available in C#: ArithmeticException, FileNotFoundException, IndexOutOfRangeException, TimeOutException, etc</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>static void checkAge(int age)
+{
+  if (age &lt; 18)
+  {
+    throw new ArithmeticException("Access denied - You must be at least 18 years old.");
+  }
+  else
+  {
+    Console.WriteLine("Access granted - You are old enough!");
+  }
+}
+static void Main(string[] args)
+{
+  checkAge(15);
+}
+//outputs System.ArithmeticException: 'Access denied - You must be at least 18 years old.'</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
         <color theme="1"/>
         <rFont val="游ゴシック"/>
         <family val="3"/>
@@ -2364,7 +3493,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="9"/>
         <color theme="1"/>
         <rFont val="游ゴシック"/>
         <family val="3"/>
@@ -2380,7 +3509,7 @@
     <r>
       <rPr>
         <b/>
-        <sz val="11"/>
+        <sz val="9"/>
         <color theme="1"/>
         <rFont val="游ゴシック"/>
         <family val="3"/>
@@ -2391,7 +3520,7 @@
     </r>
     <r>
       <rPr>
-        <sz val="11"/>
+        <sz val="9"/>
         <color theme="1"/>
         <rFont val="游ゴシック"/>
         <family val="3"/>
@@ -2411,7 +3540,704 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Class Members</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>prog2.cs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+class Car 
+{
+  public string model;
+  public string color;
+  public int year;
+  public void fullThrottle()
+  {
+    Console.WriteLine("The car is going as fast as it can!"); 
+  }
+}
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>prog.cs</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+class Program
+{
+  static void Main(string[] args)
+  {
+    Car Ford = new Car();
+    Ford.model = "Mustang";
+    Ford.color = "red";
+    Ford.year = 1969;
+    Car Opel = new Car();
+    Opel.model = "Astra";
+    Opel.color = "white";
+    Opel.year = 2005;
+    Console.WriteLine(Ford.model);
+    Console.WriteLine(Opel.model);
+  }
+}</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">With constructor:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>class Program
+{
+  static void Main(string[] args)
+  {
+    Car Ford = new Car("Mustang", "Red", 1969);
+    Car Opel = new Car("Astra", "White", 2005);
+    Console.WriteLine(Ford.model);
+    Console.WriteLine(Opel.model);
+  }
+}</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">public : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The code is accessible for all classes</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+private : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The code is only accessible within the same class</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+protected : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>The code is accessible within the same class, or in a class that is inherited from that class</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+internal : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">The code is only accessible within its own assembly, but not from another assembly
+There's also two combinations: </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>protected internal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>private protected</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: By default, all members of a class are private if you don't specify an access modifier
+class Car
+{
+  string model;  // private
+  string year;   // private
+}</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">class Person
+{
+  private string name; // field
+  public string Name   // property
+  {
+    get { return name; }   // get method
+    set { name = value; }  // set method
+  }
+}
+The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> property is associated with the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> field. It is a good practice to use the same name for both the property and the private field, but with an uppercase first letter.
+The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>get</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> method returns the value of the variable </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.
+The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>set</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> method assigns a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>name</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> variable. The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>value</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> keyword represents the value we assign to the property</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">If you try to access a sealed class, C# will generate an error
+sealed class Vehicle 
+{
+  ...
+}
+class Car : Vehicle 
+{
+  ...
+}
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">error message: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>'Car': cannot derive from sealed type 'Vehicle'</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">An abstract class can have both abstract and regular methods
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">abstract class Animal 
+{
+  public abstract void animalSound();
+  public void sleep() 
+  {
+    Console.WriteLine("Zzz");
+  }
+}
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>From the example above, it is not possible to create an object of the Animal class</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Animal myObj = new Animal(); // Will generate an error (Cannot create an instance of the abstract class or interface 'Animal')
+To access the abstract class, it must be inherited from another class. Let's convert the Animal class we used in the Polymorphism chapter to an abstract class</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">// interface
+interface Animal 
+{
+  void animalSound(); // interface method (does not have a body)
+  void run(); // interface method (does not have a body)
+}
+It is considered good practice to start with the letter "I" at the beginning of an interface, as it makes it easier for yourself and others to remember that it is an interface and not a class.
+By default, members of an interface are abstract and public.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Interfaces can contain properties and methods, but not fields</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Syntax</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+try 
+{
+  //  Block of code to try
+}
+catch (Exception e)
+{
+  //  Block of code to handle errors
+}</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>The meaning of Encapsulation, is to make sure that "sensitive" data is hidden from users. To achieve this, you must:
+--&gt;declare fields/variables as private
+--&gt;provide public get and set methods, through properties, to access and update the value of a private field</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">enum Level 
+{
+  Low,
+  Medium,
+  High
+}
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">You can access enum items with the dot syntax:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="游ゴシック"/>
+        <family val="3"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Level myVar = Level.Medium;
+Console.WriteLine(myVar);</t>
+    </r>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2419,7 +4245,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2465,6 +4291,30 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2474,7 +4324,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -2497,37 +4347,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2538,9 +4364,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2549,17 +4372,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2843,8 +4679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -2856,811 +4692,819 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="211.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="7" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="5"/>
-      <c r="B3" s="13" t="s">
+      <c r="A3" s="12"/>
+      <c r="B3" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A4" s="5"/>
-      <c r="B4" s="13" t="s">
+      <c r="A4" s="12"/>
+      <c r="B4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="56.25" x14ac:dyDescent="0.4">
-      <c r="A6" s="5"/>
-      <c r="B6" s="13" t="s">
+      <c r="A6" s="12"/>
+      <c r="B6" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="131.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="5"/>
-      <c r="B8" s="13" t="s">
+      <c r="A8" s="12"/>
+      <c r="B8" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="6" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="5"/>
-      <c r="B9" s="13" t="s">
+      <c r="A9" s="12"/>
+      <c r="B9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="2" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A10" s="5"/>
-      <c r="B10" s="13" t="s">
+      <c r="A10" s="12"/>
+      <c r="B10" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="2" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="37.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="5"/>
-      <c r="B11" s="13" t="s">
+      <c r="A11" s="12"/>
+      <c r="B11" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="2" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="93.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="5"/>
-      <c r="B12" s="15" t="s">
+      <c r="A12" s="12"/>
+      <c r="B12" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="7" t="s">
+      <c r="C12" s="3"/>
+      <c r="D12" s="2" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="112.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="6" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="56.25" x14ac:dyDescent="0.4">
-      <c r="A14" s="5"/>
-      <c r="B14" s="13" t="s">
+      <c r="A14" s="12"/>
+      <c r="B14" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="6" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="75" x14ac:dyDescent="0.4">
-      <c r="A15" s="5"/>
-      <c r="B15" s="13" t="s">
+      <c r="A15" s="12"/>
+      <c r="B15" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="6" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="75" x14ac:dyDescent="0.4">
-      <c r="A16" s="5"/>
-      <c r="B16" s="13" t="s">
+      <c r="A16" s="12"/>
+      <c r="B16" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="D16" s="6" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="93.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="7" t="s">
+      <c r="B17" s="7"/>
+      <c r="C17" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="D17" s="6" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="5"/>
-      <c r="B18" s="13" t="s">
+      <c r="A18" s="12"/>
+      <c r="B18" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="2" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="5"/>
-      <c r="B19" s="13" t="s">
+      <c r="A19" s="12"/>
+      <c r="B19" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="2" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="131.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="5"/>
-      <c r="B20" s="15" t="s">
+      <c r="A20" s="12"/>
+      <c r="B20" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="2" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="7" t="s">
+      <c r="B21" s="7"/>
+      <c r="C21" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="2" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="56.25" x14ac:dyDescent="0.4">
-      <c r="A22" s="5"/>
-      <c r="B22" s="15" t="s">
+      <c r="A22" s="12"/>
+      <c r="B22" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="2" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="131.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="B23" s="13" t="s">
+      <c r="B23" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="2" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="206.25" x14ac:dyDescent="0.4">
-      <c r="A24" s="5"/>
-      <c r="B24" s="13" t="s">
+      <c r="A24" s="12"/>
+      <c r="B24" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="2" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="112.5" x14ac:dyDescent="0.4">
-      <c r="A25" s="5"/>
-      <c r="B25" s="13" t="s">
+      <c r="A25" s="12"/>
+      <c r="B25" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="2" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="56.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="5"/>
-      <c r="B26" s="13" t="s">
+      <c r="A26" s="12"/>
+      <c r="B26" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="C26" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D26" s="7" t="s">
+      <c r="D26" s="2" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B27" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D27" s="7" t="s">
+      <c r="D27" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A28" s="5"/>
-      <c r="B28" s="13" t="s">
+      <c r="A28" s="12"/>
+      <c r="B28" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D28" s="7" t="s">
+      <c r="D28" s="2" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="5"/>
-      <c r="B29" s="13" t="s">
+      <c r="A29" s="12"/>
+      <c r="B29" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="C29" s="7" t="s">
+      <c r="C29" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="2" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="5"/>
-      <c r="B30" s="13" t="s">
+      <c r="A30" s="12"/>
+      <c r="B30" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="C30" s="7" t="s">
+      <c r="C30" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="2" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="5"/>
-      <c r="B31" s="13" t="s">
+      <c r="A31" s="12"/>
+      <c r="B31" s="7" t="s">
         <v>88</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="2" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="13"/>
-      <c r="C32" s="8" t="s">
+      <c r="B32" s="7"/>
+      <c r="C32" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="2" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="A33" s="5"/>
-      <c r="B33" s="13" t="s">
+      <c r="A33" s="12"/>
+      <c r="B33" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="C33" s="7" t="s">
+      <c r="C33" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="D33" s="7" t="s">
+      <c r="D33" s="2" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="56.25" x14ac:dyDescent="0.4">
-      <c r="A34" s="5"/>
-      <c r="B34" s="13" t="s">
+      <c r="A34" s="12"/>
+      <c r="B34" s="7" t="s">
         <v>102</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="D34" s="2" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="75" x14ac:dyDescent="0.4">
-      <c r="A35" s="5"/>
-      <c r="B35" s="13" t="s">
+      <c r="A35" s="12"/>
+      <c r="B35" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="C35" s="7" t="s">
+      <c r="C35" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D35" s="7" t="s">
+      <c r="D35" s="2" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="93.75" x14ac:dyDescent="0.4">
-      <c r="A36" s="5"/>
-      <c r="B36" s="13" t="s">
+      <c r="A36" s="12"/>
+      <c r="B36" s="7" t="s">
         <v>104</v>
       </c>
-      <c r="C36" s="7" t="s">
+      <c r="C36" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D36" s="7" t="s">
+      <c r="D36" s="2" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="56.25" x14ac:dyDescent="0.4">
-      <c r="A37" s="5"/>
-      <c r="B37" s="13" t="s">
+      <c r="A37" s="12"/>
+      <c r="B37" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="C37" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="D37" s="7" t="s">
+      <c r="D37" s="2" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="131.25" x14ac:dyDescent="0.4">
-      <c r="A38" s="5"/>
-      <c r="B38" s="13" t="s">
+      <c r="A38" s="12"/>
+      <c r="B38" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C38" s="7" t="s">
+      <c r="C38" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="2" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="150" x14ac:dyDescent="0.4">
-      <c r="A39" s="5"/>
-      <c r="B39" s="15" t="s">
+      <c r="A39" s="12"/>
+      <c r="B39" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C39" s="7" t="s">
+      <c r="C39" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D39" s="7" t="s">
+      <c r="D39" s="2" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="75" x14ac:dyDescent="0.4">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="B40" s="13" t="s">
+      <c r="B40" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="C40" s="7" t="s">
+      <c r="C40" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="D40" s="7" t="s">
+      <c r="D40" s="2" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="131.25" x14ac:dyDescent="0.4">
-      <c r="A41" s="5"/>
-      <c r="B41" s="13" t="s">
+      <c r="A41" s="12"/>
+      <c r="B41" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C41" s="7" t="s">
+      <c r="C41" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D41" s="7" t="s">
+      <c r="D41" s="2" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="112.5" x14ac:dyDescent="0.4">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="B42" s="13" t="s">
+      <c r="B42" s="7" t="s">
         <v>130</v>
       </c>
-      <c r="C42" s="7" t="s">
+      <c r="C42" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D42" s="7" t="s">
+      <c r="D42" s="2" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="187.5" x14ac:dyDescent="0.4">
-      <c r="A43" s="5"/>
-      <c r="B43" s="13" t="s">
+      <c r="A43" s="12"/>
+      <c r="B43" s="7" t="s">
         <v>133</v>
       </c>
-      <c r="C43" s="7" t="s">
+      <c r="C43" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D43" s="7" t="s">
+      <c r="D43" s="2" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="262.5" x14ac:dyDescent="0.4">
-      <c r="A44" s="5"/>
-      <c r="B44" s="13" t="s">
+      <c r="A44" s="12"/>
+      <c r="B44" s="7" t="s">
         <v>136</v>
       </c>
-      <c r="C44" s="7" t="s">
+      <c r="C44" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D44" s="7" t="s">
+      <c r="D44" s="2" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="56.25" x14ac:dyDescent="0.4">
-      <c r="A45" s="5"/>
-      <c r="B45" s="13" t="s">
+      <c r="A45" s="12"/>
+      <c r="B45" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="C45" s="7" t="s">
+      <c r="C45" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="D45" s="7" t="s">
+      <c r="D45" s="2" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="356.25" x14ac:dyDescent="0.4">
-      <c r="A46" s="5" t="s">
+      <c r="A46" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="B46" s="13"/>
-      <c r="C46" s="7" t="s">
+      <c r="B46" s="7"/>
+      <c r="C46" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D46" s="7" t="s">
+      <c r="D46" s="2" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A47" s="5"/>
-      <c r="B47" s="15" t="s">
+      <c r="A47" s="12"/>
+      <c r="B47" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="C47" s="8"/>
-      <c r="D47" s="7" t="s">
+      <c r="C47" s="3"/>
+      <c r="D47" s="2" t="s">
         <v>145</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A48" s="5"/>
-      <c r="B48" s="15" t="s">
+      <c r="A48" s="12"/>
+      <c r="B48" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="C48" s="8"/>
-      <c r="D48" s="7" t="s">
+      <c r="C48" s="3"/>
+      <c r="D48" s="2" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="A49" s="5" t="s">
+      <c r="A49" s="12" t="s">
         <v>149</v>
       </c>
-      <c r="B49" s="13" t="s">
+      <c r="B49" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="C49" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="D49" s="7" t="s">
+      <c r="D49" s="2" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="112.5" x14ac:dyDescent="0.4">
-      <c r="A50" s="5"/>
-      <c r="B50" s="13" t="s">
+      <c r="A50" s="12"/>
+      <c r="B50" s="7" t="s">
         <v>153</v>
       </c>
-      <c r="C50" s="7" t="s">
+      <c r="C50" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D50" s="7" t="s">
+      <c r="D50" s="2" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="187.5" x14ac:dyDescent="0.4">
-      <c r="A51" s="5"/>
-      <c r="B51" s="13" t="s">
+      <c r="A51" s="12"/>
+      <c r="B51" s="7" t="s">
         <v>156</v>
       </c>
-      <c r="C51" s="7" t="s">
+      <c r="C51" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="D51" s="7" t="s">
+      <c r="D51" s="2" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="75" x14ac:dyDescent="0.4">
-      <c r="A52" s="5" t="s">
+      <c r="A52" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="B52" s="13"/>
-      <c r="C52" s="7" t="s">
+      <c r="B52" s="7"/>
+      <c r="C52" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="D52" s="7" t="s">
+      <c r="D52" s="2" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="75" x14ac:dyDescent="0.4">
-      <c r="A53" s="5"/>
-      <c r="B53" s="13" t="s">
+      <c r="A53" s="12"/>
+      <c r="B53" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="C53" s="7" t="s">
+      <c r="C53" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="D53" s="7" t="s">
+      <c r="D53" s="2" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="112.5" x14ac:dyDescent="0.4">
-      <c r="A54" s="5"/>
-      <c r="B54" s="13" t="s">
+      <c r="A54" s="12"/>
+      <c r="B54" s="7" t="s">
         <v>164</v>
       </c>
-      <c r="C54" s="7" t="s">
+      <c r="C54" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="D54" s="7" t="s">
+      <c r="D54" s="2" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="150" x14ac:dyDescent="0.4">
-      <c r="A55" s="5" t="s">
+      <c r="A55" s="12" t="s">
         <v>168</v>
       </c>
-      <c r="B55" s="13" t="s">
+      <c r="B55" s="7" t="s">
         <v>169</v>
       </c>
-      <c r="C55" s="7" t="s">
+      <c r="C55" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="D55" s="7" t="s">
+      <c r="D55" s="2" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="150" x14ac:dyDescent="0.4">
-      <c r="A56" s="5"/>
-      <c r="B56" s="13" t="s">
+      <c r="A56" s="12"/>
+      <c r="B56" s="7" t="s">
         <v>172</v>
       </c>
-      <c r="C56" s="7" t="s">
+      <c r="C56" s="2" t="s">
         <v>173</v>
       </c>
-      <c r="D56" s="7" t="s">
+      <c r="D56" s="2" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="56.25" x14ac:dyDescent="0.4">
-      <c r="A57" s="5" t="s">
+      <c r="A57" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="B57" s="13" t="s">
+      <c r="B57" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="C57" s="7" t="s">
+      <c r="C57" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="D57" s="7" t="s">
+      <c r="D57" s="2" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="56.25" x14ac:dyDescent="0.4">
-      <c r="A58" s="5"/>
-      <c r="B58" s="15" t="s">
+      <c r="A58" s="12"/>
+      <c r="B58" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="C58" s="7" t="s">
+      <c r="C58" s="2" t="s">
         <v>180</v>
       </c>
-      <c r="D58" s="7" t="s">
+      <c r="D58" s="2" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="75" x14ac:dyDescent="0.4">
-      <c r="A59" s="5"/>
-      <c r="B59" s="15" t="s">
+      <c r="A59" s="12"/>
+      <c r="B59" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="C59" s="7" t="s">
+      <c r="C59" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="D59" s="7" t="s">
+      <c r="D59" s="2" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="56.25" x14ac:dyDescent="0.4">
-      <c r="A60" s="5"/>
-      <c r="B60" s="13" t="s">
+      <c r="A60" s="12"/>
+      <c r="B60" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="C60" s="7" t="s">
+      <c r="C60" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="D60" s="7" t="s">
+      <c r="D60" s="2" t="s">
         <v>187</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="93.75" x14ac:dyDescent="0.4">
-      <c r="A61" s="5"/>
-      <c r="B61" s="13" t="s">
+      <c r="A61" s="12"/>
+      <c r="B61" s="7" t="s">
         <v>188</v>
       </c>
-      <c r="C61" s="7" t="s">
+      <c r="C61" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="D61" s="7" t="s">
+      <c r="D61" s="2" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="93.75" x14ac:dyDescent="0.4">
-      <c r="A62" s="5"/>
-      <c r="B62" s="13" t="s">
+      <c r="A62" s="12"/>
+      <c r="B62" s="7" t="s">
         <v>191</v>
       </c>
-      <c r="C62" s="7" t="s">
+      <c r="C62" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="D62" s="7" t="s">
+      <c r="D62" s="2" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="131.25" x14ac:dyDescent="0.4">
-      <c r="A63" s="5"/>
-      <c r="B63" s="13" t="s">
+      <c r="A63" s="12"/>
+      <c r="B63" s="7" t="s">
         <v>192</v>
       </c>
-      <c r="C63" s="7" t="s">
+      <c r="C63" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="D63" s="7" t="s">
+      <c r="D63" s="2" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="281.25" x14ac:dyDescent="0.4">
-      <c r="A64" s="5"/>
-      <c r="B64" s="13" t="s">
+      <c r="A64" s="12"/>
+      <c r="B64" s="7" t="s">
         <v>195</v>
       </c>
-      <c r="C64" s="7" t="s">
+      <c r="C64" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="D64" s="11" t="s">
+      <c r="D64" s="6" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="337.5" x14ac:dyDescent="0.4">
-      <c r="A65" s="5"/>
+      <c r="A65" s="12"/>
       <c r="B65" s="12" t="s">
         <v>198</v>
       </c>
-      <c r="C65" s="7" t="s">
+      <c r="C65" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="D65" s="7" t="s">
+      <c r="D65" s="2" t="s">
         <v>201</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="5"/>
+      <c r="A66" s="12"/>
       <c r="B66" s="12"/>
-      <c r="C66" s="7"/>
-      <c r="D66" s="7" t="s">
+      <c r="C66" s="2"/>
+      <c r="D66" s="2" t="s">
         <v>199</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A7:A12"/>
+    <mergeCell ref="A27:A31"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A23:A26"/>
     <mergeCell ref="A52:A54"/>
     <mergeCell ref="A55:A56"/>
     <mergeCell ref="A57:A66"/>
@@ -3670,14 +5514,6 @@
     <mergeCell ref="A42:A45"/>
     <mergeCell ref="A46:A48"/>
     <mergeCell ref="A49:A51"/>
-    <mergeCell ref="A27:A31"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="A21:A22"/>
-    <mergeCell ref="A23:A26"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A2:A4"/>
-    <mergeCell ref="A7:A12"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3689,149 +5525,149 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView topLeftCell="C16" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="19.25" customWidth="1"/>
-    <col min="2" max="2" width="23.625" customWidth="1"/>
-    <col min="3" max="3" width="51.25" customWidth="1"/>
-    <col min="4" max="4" width="81.125" customWidth="1"/>
+    <col min="1" max="1" width="15.625" customWidth="1"/>
+    <col min="2" max="2" width="18.625" customWidth="1"/>
+    <col min="3" max="3" width="66.875" customWidth="1"/>
+    <col min="4" max="4" width="74.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="75" x14ac:dyDescent="0.4">
-      <c r="A2" s="19" t="s">
+    <row r="2" spans="1:4" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A2" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="B2" s="13"/>
-      <c r="C2" s="7" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="2" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="131.25" x14ac:dyDescent="0.4">
-      <c r="A3" s="19"/>
-      <c r="B3" s="13" t="s">
+      <c r="A3" s="17"/>
+      <c r="B3" s="7" t="s">
         <v>204</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="2" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="168.75" x14ac:dyDescent="0.4">
-      <c r="A4" s="19"/>
-      <c r="B4" s="13" t="s">
+      <c r="A4" s="17"/>
+      <c r="B4" s="7" t="s">
         <v>207</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="2" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="243.75" x14ac:dyDescent="0.4">
-      <c r="A5" s="19" t="s">
+      <c r="A5" s="17" t="s">
         <v>211</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="9" t="s">
         <v>210</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="2" t="s">
         <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="206.25" x14ac:dyDescent="0.4">
-      <c r="A6" s="19"/>
-      <c r="B6" s="15" t="s">
+      <c r="A6" s="17"/>
+      <c r="B6" s="9" t="s">
         <v>214</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="2" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="243.75" x14ac:dyDescent="0.4">
-      <c r="A7" s="19"/>
-      <c r="B7" s="13" t="s">
+      <c r="A7" s="17"/>
+      <c r="B7" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="2" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="168.75" x14ac:dyDescent="0.4">
-      <c r="A8" s="19"/>
-      <c r="B8" s="13" t="s">
+      <c r="A8" s="17"/>
+      <c r="B8" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="10" t="s">
         <v>222</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="2" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="168.75" x14ac:dyDescent="0.4">
-      <c r="A9" s="19"/>
-      <c r="B9" s="5" t="s">
+      <c r="A9" s="17"/>
+      <c r="B9" s="11" t="s">
         <v>223</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="2" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="187.5" x14ac:dyDescent="0.4">
-      <c r="A10" s="19"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="7" t="s">
+      <c r="A10" s="17"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="2" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="281.25" x14ac:dyDescent="0.4">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="7" t="s">
+      <c r="B11" s="7"/>
+      <c r="C11" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="2" t="s">
         <v>230</v>
       </c>
     </row>
@@ -3849,134 +5685,621 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="15.375" customWidth="1"/>
     <col min="2" max="2" width="30.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.25" customWidth="1"/>
-    <col min="4" max="4" width="67.875" customWidth="1"/>
+    <col min="3" max="3" width="51.625" customWidth="1"/>
+    <col min="4" max="4" width="80.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="150" x14ac:dyDescent="0.4">
-      <c r="A2" s="16" t="s">
+    <row r="2" spans="1:4" ht="99" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="12" t="s">
         <v>232</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="14" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="37.5" x14ac:dyDescent="0.4">
-      <c r="A3" s="3"/>
-      <c r="B3" t="s">
+      <c r="A3" s="12"/>
+      <c r="B3" s="7" t="s">
         <v>236</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="14" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="75" x14ac:dyDescent="0.4">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:4" ht="63.75" x14ac:dyDescent="0.4">
+      <c r="A4" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" s="14" t="s">
         <v>240</v>
       </c>
-      <c r="C4" s="1" t="s">
+    </row>
+    <row r="5" spans="1:4" ht="63.75" x14ac:dyDescent="0.4">
+      <c r="A5" s="12"/>
+      <c r="B5" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="C5" s="10" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="75" x14ac:dyDescent="0.4">
-      <c r="A5" s="3"/>
-      <c r="B5" t="s">
+      <c r="D5" s="14" t="s">
         <v>243</v>
       </c>
-      <c r="C5" s="17" t="s">
+    </row>
+    <row r="6" spans="1:4" ht="142.5" x14ac:dyDescent="0.4">
+      <c r="A6" s="12"/>
+      <c r="B6" s="7" t="s">
         <v>244</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="C6" s="10" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="168.75" x14ac:dyDescent="0.4">
-      <c r="A6" s="3"/>
-      <c r="B6" t="s">
+      <c r="D6" s="14" t="s">
         <v>246</v>
       </c>
-      <c r="C6" s="17" t="s">
+    </row>
+    <row r="7" spans="1:4" ht="174" x14ac:dyDescent="0.4">
+      <c r="A7" s="12"/>
+      <c r="B7" s="7" t="s">
         <v>247</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="C7" s="10" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="206.25" x14ac:dyDescent="0.4">
-      <c r="A7" s="3"/>
-      <c r="B7" t="s">
+      <c r="D7" s="14" t="s">
         <v>249</v>
       </c>
-      <c r="C7" s="17" t="s">
+    </row>
+    <row r="8" spans="1:4" ht="221.25" x14ac:dyDescent="0.4">
+      <c r="A8" s="12"/>
+      <c r="B8" s="7" t="s">
         <v>250</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="C8" s="2" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="261.75" x14ac:dyDescent="0.4">
-      <c r="A8" s="3"/>
-      <c r="B8" t="s">
+      <c r="D8" s="15" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="174" x14ac:dyDescent="0.4">
+      <c r="A9" s="12" t="s">
         <v>252</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="B9" s="7"/>
+      <c r="C9" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D9" s="14" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A9" t="s">
+    <row r="10" spans="1:4" ht="189.75" x14ac:dyDescent="0.4">
+      <c r="A10" s="12"/>
+      <c r="B10" s="11" t="s">
         <v>255</v>
       </c>
+      <c r="C10" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="205.5" x14ac:dyDescent="0.4">
+      <c r="A11" s="12"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="300" x14ac:dyDescent="0.4">
+      <c r="A12" s="12"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="221.25" x14ac:dyDescent="0.4">
+      <c r="A13" s="12"/>
+      <c r="B13" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="409.6" x14ac:dyDescent="0.4">
+      <c r="A14" s="12"/>
+      <c r="B14" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="262.5" x14ac:dyDescent="0.4">
+      <c r="A15" s="12" t="s">
+        <v>267</v>
+      </c>
+      <c r="B15" s="7"/>
+      <c r="C15" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="237" x14ac:dyDescent="0.4">
+      <c r="A16" s="12"/>
+      <c r="B16" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="300" x14ac:dyDescent="0.4">
+      <c r="A17" s="12"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="D17" s="14" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="318.75" x14ac:dyDescent="0.4">
+      <c r="A18" s="12"/>
+      <c r="B18" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>276</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="79.5" x14ac:dyDescent="0.4">
+      <c r="A19" s="12" t="s">
+        <v>278</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="142.5" x14ac:dyDescent="0.4">
+      <c r="A20" s="12"/>
+      <c r="B20" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>282</v>
+      </c>
+      <c r="D20" s="14" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="189.75" x14ac:dyDescent="0.4">
+      <c r="A21" s="12"/>
+      <c r="B21" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="D21" s="14" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="111" x14ac:dyDescent="0.4">
+      <c r="A22" s="12"/>
+      <c r="B22" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>287</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="112.5" x14ac:dyDescent="0.4">
+      <c r="A23" s="12" t="s">
+        <v>288</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="D23" s="16"/>
+    </row>
+    <row r="24" spans="1:4" ht="221.25" x14ac:dyDescent="0.4">
+      <c r="A24" s="12"/>
+      <c r="B24" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D24" s="14" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="300" x14ac:dyDescent="0.4">
+      <c r="A25" s="12"/>
+      <c r="B25" s="7"/>
+      <c r="C25" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="237" x14ac:dyDescent="0.4">
+      <c r="A26" s="12"/>
+      <c r="B26" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>295</v>
+      </c>
+      <c r="D26" s="14" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="378.75" x14ac:dyDescent="0.4">
+      <c r="A27" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="32.25" x14ac:dyDescent="0.4">
+      <c r="A28" s="12"/>
+      <c r="B28" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="15" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="174" x14ac:dyDescent="0.4">
+      <c r="A29" s="12"/>
+      <c r="B29" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="331.5" x14ac:dyDescent="0.4">
+      <c r="A30" s="12" t="s">
+        <v>305</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="409.6" x14ac:dyDescent="0.4">
+      <c r="A31" s="12"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="2" t="s">
+        <v>309</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="409.6" x14ac:dyDescent="0.4">
+      <c r="A32" s="12"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="243.75" x14ac:dyDescent="0.4">
+      <c r="A33" s="12" t="s">
+        <v>313</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>315</v>
+      </c>
+      <c r="D33" s="15" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="409.6" x14ac:dyDescent="0.4">
+      <c r="A34" s="12"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="13" t="s">
+        <v>317</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="158.25" x14ac:dyDescent="0.4">
+      <c r="A35" s="12" t="s">
+        <v>318</v>
+      </c>
+      <c r="B35" s="7"/>
+      <c r="C35" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="409.6" x14ac:dyDescent="0.4">
+      <c r="A36" s="12"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="409.6" x14ac:dyDescent="0.4">
+      <c r="A37" s="12"/>
+      <c r="B37" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="D37" s="14" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="158.25" x14ac:dyDescent="0.4">
+      <c r="A38" s="12" t="s">
+        <v>325</v>
+      </c>
+      <c r="B38" s="7"/>
+      <c r="C38" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="D38" s="14" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="237" x14ac:dyDescent="0.4">
+      <c r="A39" s="12"/>
+      <c r="B39" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="D39" s="14" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="252.75" x14ac:dyDescent="0.4">
+      <c r="A40" s="12"/>
+      <c r="B40" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="D40" s="14" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="363" x14ac:dyDescent="0.4">
+      <c r="A41" s="12"/>
+      <c r="B41" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="126.75" x14ac:dyDescent="0.4">
+      <c r="A42" s="12" t="s">
+        <v>336</v>
+      </c>
+      <c r="B42" s="7" t="s">
+        <v>337</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="111" x14ac:dyDescent="0.4">
+      <c r="A43" s="12"/>
+      <c r="B43" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="56.25" x14ac:dyDescent="0.4">
+      <c r="A44" s="12" t="s">
+        <v>343</v>
+      </c>
+      <c r="B44" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="142.5" x14ac:dyDescent="0.4">
+      <c r="A45" s="12"/>
+      <c r="B45" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="158.25" x14ac:dyDescent="0.4">
+      <c r="A46" s="12"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="D46" s="14" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="158.25" x14ac:dyDescent="0.4">
+      <c r="A47" s="12"/>
+      <c r="B47" s="7"/>
+      <c r="C47" s="6" t="s">
+        <v>351</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="221.25" x14ac:dyDescent="0.4">
+      <c r="A48" s="12"/>
+      <c r="B48" s="7" t="s">
+        <v>353</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="252.75" x14ac:dyDescent="0.4">
+      <c r="A49" s="12"/>
+      <c r="B49" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>358</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="14">
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="A38:A41"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="A44:A49"/>
+    <mergeCell ref="A19:A22"/>
+    <mergeCell ref="A23:A26"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="A33:A34"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="A4:A8"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="A15:A18"/>
+    <mergeCell ref="A9:A14"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
C# Studing material final updated
</commit_message>
<xml_diff>
--- a/C#.xlsx
+++ b/C#.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Basics" sheetId="1" r:id="rId1"/>
@@ -1451,15 +1451,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>\'          '                Single quote
-\"         "                Double quote
-\\        \                Backslash
-\n                          New Line 
-\t                           Tab 
-\b                          Backspace</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">string txt = "We are the so-called \"Vikings\" from the north.";
 string txt = "It\'s alright.";
 string txt = "The character \\ is called backslash.";
@@ -4238,6 +4229,15 @@
       <t>Level myVar = Level.Medium;
 Console.WriteLine(myVar);</t>
     </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>\'          '                Single quote
+\"         "                Double quote
+\\        \                Backslash
+\n(or)\x0A            New Line 
+\t                           Tab 
+\b                          Backspace</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -4679,8 +4679,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A66"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -5151,10 +5151,10 @@
         <v>106</v>
       </c>
       <c r="C38" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="D38" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="150" x14ac:dyDescent="0.4">
@@ -5163,328 +5163,328 @@
         <v>107</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="75" x14ac:dyDescent="0.4">
       <c r="A40" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B40" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="B40" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="C40" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>123</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="131.25" x14ac:dyDescent="0.4">
       <c r="A41" s="12"/>
       <c r="B41" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C41" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D41" s="2" t="s">
         <v>127</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="112.5" x14ac:dyDescent="0.4">
       <c r="A42" s="12" t="s">
+        <v>128</v>
+      </c>
+      <c r="B42" s="7" t="s">
         <v>129</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="C42" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="D42" s="2" t="s">
         <v>131</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="187.5" x14ac:dyDescent="0.4">
       <c r="A43" s="12"/>
       <c r="B43" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="262.5" x14ac:dyDescent="0.4">
       <c r="A44" s="12"/>
       <c r="B44" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A45" s="12"/>
       <c r="B45" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>140</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="356.25" x14ac:dyDescent="0.4">
       <c r="A46" s="12" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B46" s="7"/>
       <c r="C46" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A47" s="12"/>
       <c r="B47" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A48" s="12"/>
       <c r="B48" s="9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C48" s="3"/>
       <c r="D48" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A49" s="12" t="s">
+        <v>148</v>
+      </c>
+      <c r="B49" s="7" t="s">
         <v>149</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="C49" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="D49" s="2" t="s">
         <v>151</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="112.5" x14ac:dyDescent="0.4">
       <c r="A50" s="12"/>
       <c r="B50" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="C50" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="D50" s="2" t="s">
         <v>154</v>
-      </c>
-      <c r="D50" s="2" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="187.5" x14ac:dyDescent="0.4">
       <c r="A51" s="12"/>
       <c r="B51" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C51" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="D51" s="2" t="s">
         <v>157</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="75" x14ac:dyDescent="0.4">
       <c r="A52" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B52" s="7"/>
       <c r="C52" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="75" x14ac:dyDescent="0.4">
       <c r="A53" s="12"/>
       <c r="B53" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C53" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>162</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="112.5" x14ac:dyDescent="0.4">
       <c r="A54" s="12"/>
       <c r="B54" s="7" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="150" x14ac:dyDescent="0.4">
       <c r="A55" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="B55" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="B55" s="7" t="s">
+      <c r="C55" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="D55" s="2" t="s">
         <v>170</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="150" x14ac:dyDescent="0.4">
       <c r="A56" s="12"/>
       <c r="B56" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="D56" s="2" t="s">
         <v>173</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A57" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="B57" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="B57" s="7" t="s">
+      <c r="C57" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C57" s="2" t="s">
+      <c r="D57" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A58" s="12"/>
       <c r="B58" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>179</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="D58" s="2" t="s">
         <v>180</v>
-      </c>
-      <c r="D58" s="2" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="75" x14ac:dyDescent="0.4">
       <c r="A59" s="12"/>
       <c r="B59" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="C59" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="C59" s="2" t="s">
+      <c r="D59" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A60" s="12"/>
       <c r="B60" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>185</v>
       </c>
-      <c r="C60" s="2" t="s">
+      <c r="D60" s="2" t="s">
         <v>186</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="93.75" x14ac:dyDescent="0.4">
       <c r="A61" s="12"/>
       <c r="B61" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="C61" s="2" t="s">
+      <c r="D61" s="2" t="s">
         <v>189</v>
-      </c>
-      <c r="D61" s="2" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="93.75" x14ac:dyDescent="0.4">
       <c r="A62" s="12"/>
       <c r="B62" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C62" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D62" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="131.25" x14ac:dyDescent="0.4">
       <c r="A63" s="12"/>
       <c r="B63" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>192</v>
       </c>
-      <c r="C63" s="2" t="s">
+      <c r="D63" s="2" t="s">
         <v>193</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="281.25" x14ac:dyDescent="0.4">
       <c r="A64" s="12"/>
       <c r="B64" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D64" s="6" t="s">
         <v>195</v>
-      </c>
-      <c r="C64" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="D64" s="6" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="337.5" x14ac:dyDescent="0.4">
       <c r="A65" s="12"/>
       <c r="B65" s="12" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C65" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D65" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.4">
@@ -5492,7 +5492,7 @@
       <c r="B66" s="12"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -5525,8 +5525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView topLeftCell="B2" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -5553,122 +5553,122 @@
     </row>
     <row r="2" spans="1:4" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A2" s="17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B2" s="7"/>
       <c r="C2" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="131.25" x14ac:dyDescent="0.4">
       <c r="A3" s="17"/>
       <c r="B3" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>205</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="168.75" x14ac:dyDescent="0.4">
       <c r="A4" s="17"/>
       <c r="B4" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>208</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="243.75" x14ac:dyDescent="0.4">
       <c r="A5" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="C5" s="2" t="s">
+      <c r="D5" s="2" t="s">
         <v>212</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="206.25" x14ac:dyDescent="0.4">
       <c r="A6" s="17"/>
       <c r="B6" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="D6" s="2" t="s">
         <v>215</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="243.75" x14ac:dyDescent="0.4">
       <c r="A7" s="17"/>
       <c r="B7" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>217</v>
-      </c>
-      <c r="C7" s="10" t="s">
-        <v>219</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="168.75" x14ac:dyDescent="0.4">
       <c r="A8" s="17"/>
       <c r="B8" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>220</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="168.75" x14ac:dyDescent="0.4">
       <c r="A9" s="17"/>
       <c r="B9" s="11" t="s">
+        <v>222</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>224</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="187.5" x14ac:dyDescent="0.4">
       <c r="A10" s="17"/>
       <c r="B10" s="11"/>
       <c r="C10" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>226</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="281.25" x14ac:dyDescent="0.4">
       <c r="A11" s="18" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B11" s="7"/>
       <c r="C11" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>229</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -5688,7 +5688,7 @@
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -5715,570 +5715,570 @@
     </row>
     <row r="2" spans="1:4" ht="99" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="B2" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="C2" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="14" t="s">
         <v>234</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="37.5" x14ac:dyDescent="0.4">
       <c r="A3" s="12"/>
       <c r="B3" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="14" t="s">
         <v>237</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="63.75" x14ac:dyDescent="0.4">
       <c r="A4" s="12" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B4" s="7"/>
       <c r="C4" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="D4" s="14" t="s">
         <v>239</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="63.75" x14ac:dyDescent="0.4">
       <c r="A5" s="12"/>
       <c r="B5" s="7" t="s">
+        <v>240</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="D5" s="14" t="s">
         <v>242</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="142.5" x14ac:dyDescent="0.4">
       <c r="A6" s="12"/>
       <c r="B6" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C6" s="10" t="s">
+      <c r="D6" s="14" t="s">
         <v>245</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="174" x14ac:dyDescent="0.4">
       <c r="A7" s="12"/>
       <c r="B7" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>247</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="D7" s="14" t="s">
         <v>248</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="221.25" x14ac:dyDescent="0.4">
       <c r="A8" s="12"/>
       <c r="B8" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>251</v>
-      </c>
       <c r="D8" s="15" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="174" x14ac:dyDescent="0.4">
       <c r="A9" s="12" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B9" s="7"/>
       <c r="C9" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="D9" s="14" t="s">
         <v>253</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>254</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="189.75" x14ac:dyDescent="0.4">
       <c r="A10" s="12"/>
       <c r="B10" s="11" t="s">
+        <v>254</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="14" t="s">
         <v>256</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>257</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="205.5" x14ac:dyDescent="0.4">
       <c r="A11" s="12"/>
       <c r="B11" s="11"/>
       <c r="C11" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="D11" s="14" t="s">
         <v>258</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="300" x14ac:dyDescent="0.4">
       <c r="A12" s="12"/>
       <c r="B12" s="11"/>
       <c r="C12" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="D12" s="14" t="s">
         <v>260</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="221.25" x14ac:dyDescent="0.4">
       <c r="A13" s="12"/>
       <c r="B13" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>262</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="14" t="s">
         <v>263</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="409.6" x14ac:dyDescent="0.4">
       <c r="A14" s="12"/>
       <c r="B14" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>265</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>266</v>
-      </c>
       <c r="D14" s="15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="262.5" x14ac:dyDescent="0.4">
       <c r="A15" s="12" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="237" x14ac:dyDescent="0.4">
       <c r="A16" s="12"/>
       <c r="B16" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>270</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="14" t="s">
         <v>271</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>272</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="300" x14ac:dyDescent="0.4">
       <c r="A17" s="12"/>
       <c r="B17" s="7"/>
       <c r="C17" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="318.75" x14ac:dyDescent="0.4">
       <c r="A18" s="12"/>
       <c r="B18" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>275</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>276</v>
-      </c>
       <c r="D18" s="15" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="79.5" x14ac:dyDescent="0.4">
       <c r="A19" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="C19" s="6" t="s">
         <v>278</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>279</v>
-      </c>
       <c r="D19" s="15" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="142.5" x14ac:dyDescent="0.4">
       <c r="A20" s="12"/>
       <c r="B20" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="D20" s="14" t="s">
         <v>280</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>282</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="189.75" x14ac:dyDescent="0.4">
       <c r="A21" s="12"/>
       <c r="B21" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="C21" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="D21" s="14" t="s">
         <v>284</v>
-      </c>
-      <c r="D21" s="14" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="111" x14ac:dyDescent="0.4">
       <c r="A22" s="12"/>
       <c r="B22" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="C22" s="2" t="s">
-        <v>287</v>
-      </c>
       <c r="D22" s="15" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="112.5" x14ac:dyDescent="0.4">
       <c r="A23" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>288</v>
       </c>
-      <c r="B23" s="7" t="s">
-        <v>289</v>
-      </c>
       <c r="C23" s="2" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D23" s="16"/>
     </row>
     <row r="24" spans="1:4" ht="221.25" x14ac:dyDescent="0.4">
       <c r="A24" s="12"/>
       <c r="B24" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>290</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>291</v>
-      </c>
       <c r="D24" s="14" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="300" x14ac:dyDescent="0.4">
       <c r="A25" s="12"/>
       <c r="B25" s="7"/>
       <c r="C25" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="D25" s="14" t="s">
         <v>292</v>
-      </c>
-      <c r="D25" s="14" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="237" x14ac:dyDescent="0.4">
       <c r="A26" s="12"/>
       <c r="B26" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>294</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="D26" s="14" t="s">
         <v>295</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="378.75" x14ac:dyDescent="0.4">
       <c r="A27" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>297</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="C27" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="14" t="s">
         <v>299</v>
-      </c>
-      <c r="D27" s="14" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="32.25" x14ac:dyDescent="0.4">
       <c r="A28" s="12"/>
       <c r="B28" s="7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="15" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="174" x14ac:dyDescent="0.4">
       <c r="A29" s="12"/>
       <c r="B29" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>304</v>
-      </c>
       <c r="D29" s="14" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="331.5" x14ac:dyDescent="0.4">
       <c r="A30" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="B30" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="B30" s="7" t="s">
+      <c r="C30" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="D30" s="14" t="s">
         <v>307</v>
-      </c>
-      <c r="D30" s="14" t="s">
-        <v>308</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="409.6" x14ac:dyDescent="0.4">
       <c r="A31" s="12"/>
       <c r="B31" s="7"/>
       <c r="C31" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="D31" s="14" t="s">
         <v>309</v>
-      </c>
-      <c r="D31" s="14" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="409.6" x14ac:dyDescent="0.4">
       <c r="A32" s="12"/>
       <c r="B32" s="7"/>
       <c r="C32" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D32" s="14" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="243.75" x14ac:dyDescent="0.4">
       <c r="A33" s="12" t="s">
+        <v>312</v>
+      </c>
+      <c r="B33" s="7" t="s">
         <v>313</v>
       </c>
-      <c r="B33" s="7" t="s">
+      <c r="C33" s="2" t="s">
         <v>314</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>315</v>
-      </c>
       <c r="D33" s="15" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="409.6" x14ac:dyDescent="0.4">
       <c r="A34" s="12"/>
       <c r="B34" s="7"/>
       <c r="C34" s="13" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D34" s="14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="158.25" x14ac:dyDescent="0.4">
       <c r="A35" s="12" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B35" s="7"/>
       <c r="C35" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D35" s="14" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="409.6" x14ac:dyDescent="0.4">
       <c r="A36" s="12"/>
       <c r="B36" s="7"/>
       <c r="C36" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="D36" s="14" t="s">
         <v>320</v>
-      </c>
-      <c r="D36" s="14" t="s">
-        <v>321</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="409.6" x14ac:dyDescent="0.4">
       <c r="A37" s="12"/>
       <c r="B37" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>322</v>
       </c>
-      <c r="C37" s="2" t="s">
+      <c r="D37" s="14" t="s">
         <v>323</v>
-      </c>
-      <c r="D37" s="14" t="s">
-        <v>324</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="158.25" x14ac:dyDescent="0.4">
       <c r="A38" s="12" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B38" s="7"/>
       <c r="C38" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D38" s="14" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="237" x14ac:dyDescent="0.4">
       <c r="A39" s="12"/>
       <c r="B39" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="C39" s="2" t="s">
         <v>327</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="D39" s="14" t="s">
         <v>328</v>
-      </c>
-      <c r="D39" s="14" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="252.75" x14ac:dyDescent="0.4">
       <c r="A40" s="12"/>
       <c r="B40" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="C40" s="2" t="s">
         <v>330</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="D40" s="14" t="s">
         <v>331</v>
-      </c>
-      <c r="D40" s="14" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="363" x14ac:dyDescent="0.4">
       <c r="A41" s="12"/>
       <c r="B41" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="D41" s="14" t="s">
         <v>333</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>335</v>
-      </c>
-      <c r="D41" s="14" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="126.75" x14ac:dyDescent="0.4">
       <c r="A42" s="12" t="s">
+        <v>335</v>
+      </c>
+      <c r="B42" s="7" t="s">
         <v>336</v>
       </c>
-      <c r="B42" s="7" t="s">
+      <c r="C42" s="2" t="s">
         <v>337</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="D42" s="14" t="s">
         <v>338</v>
-      </c>
-      <c r="D42" s="14" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="111" x14ac:dyDescent="0.4">
       <c r="A43" s="12"/>
       <c r="B43" s="7" t="s">
+        <v>339</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="C43" s="2" t="s">
+      <c r="D43" s="14" t="s">
         <v>341</v>
-      </c>
-      <c r="D43" s="14" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="56.25" x14ac:dyDescent="0.4">
       <c r="A44" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="B44" s="7" t="s">
         <v>343</v>
       </c>
-      <c r="B44" s="7" t="s">
-        <v>344</v>
-      </c>
       <c r="C44" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="D44" s="14" t="s">
         <v>346</v>
-      </c>
-      <c r="D44" s="14" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="142.5" x14ac:dyDescent="0.4">
       <c r="A45" s="12"/>
       <c r="B45" s="7" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D45" s="15" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="158.25" x14ac:dyDescent="0.4">
       <c r="A46" s="12"/>
       <c r="B46" s="7"/>
       <c r="C46" s="6" t="s">
+        <v>348</v>
+      </c>
+      <c r="D46" s="14" t="s">
         <v>349</v>
-      </c>
-      <c r="D46" s="14" t="s">
-        <v>350</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="158.25" x14ac:dyDescent="0.4">
       <c r="A47" s="12"/>
       <c r="B47" s="7"/>
       <c r="C47" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="D47" s="14" t="s">
         <v>351</v>
-      </c>
-      <c r="D47" s="14" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="221.25" x14ac:dyDescent="0.4">
       <c r="A48" s="12"/>
       <c r="B48" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="C48" s="6" t="s">
         <v>353</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="D48" s="14" t="s">
         <v>354</v>
-      </c>
-      <c r="D48" s="14" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="252.75" x14ac:dyDescent="0.4">
       <c r="A49" s="12"/>
       <c r="B49" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>356</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="D49" s="14" t="s">
         <v>357</v>
-      </c>
-      <c r="D49" s="14" t="s">
-        <v>358</v>
       </c>
     </row>
   </sheetData>

</xml_diff>